<commit_message>
Clean quiz banks, merge LOGIK into 500-set, and add audit tooling
</commit_message>
<xml_diff>
--- a/QuizBank/quiz_bank_W_Fragen_spaced_210_DE_ONLY.xlsx
+++ b/QuizBank/quiz_bank_W_Fragen_spaced_210_DE_ONLY.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="quiz_bank" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="quiz_bank" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1236,7 +1236,7 @@
       </c>
       <c r="J11" s="2" t="inlineStr">
         <is>
-          <t>„Wen“ fragt nach dem Akkusativ-Objekt (Person/Sache).</t>
+          <t>„Wen“ fragt nach einer Person im Akkusativ.</t>
         </is>
       </c>
       <c r="K11" s="2" t="inlineStr">
@@ -2685,7 +2685,7 @@
       </c>
       <c r="J32" s="2" t="inlineStr">
         <is>
-          <t>„Wen“ fragt nach dem Akkusativ-Objekt (Person/Sache).</t>
+          <t>„Wen“ fragt nach einer Person im Akkusativ.</t>
         </is>
       </c>
       <c r="K32" s="2" t="inlineStr">
@@ -3135,7 +3135,7 @@
       </c>
       <c r="C39" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">_____ arbeitest du? </t>
+          <t>_____ arbeitest du gerade im Projekt?</t>
         </is>
       </c>
       <c r="D39" s="2" t="inlineStr">
@@ -3204,7 +3204,7 @@
       </c>
       <c r="C40" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">_____ brauchst du das? </t>
+          <t>_____ brauchst du diese Funktion?</t>
         </is>
       </c>
       <c r="D40" s="2" t="inlineStr">
@@ -4134,7 +4134,7 @@
       </c>
       <c r="J53" s="2" t="inlineStr">
         <is>
-          <t>„Wen“ fragt nach dem Akkusativ-Objekt (Person/Sache).</t>
+          <t>„Wen“ fragt nach einer Person im Akkusativ.</t>
         </is>
       </c>
       <c r="K53" s="2" t="inlineStr">
@@ -4446,7 +4446,7 @@
       </c>
       <c r="C58" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">_____ schreibst du? </t>
+          <t>_____ schreibst du in deinem Bericht?</t>
         </is>
       </c>
       <c r="D58" s="2" t="inlineStr">
@@ -4658,7 +4658,7 @@
       </c>
       <c r="D61" s="2" t="inlineStr">
         <is>
-          <t>Wie</t>
+          <t>Wer</t>
         </is>
       </c>
       <c r="E61" s="2" t="inlineStr">
@@ -4673,7 +4673,7 @@
       </c>
       <c r="G61" s="2" t="inlineStr">
         <is>
-          <t>Warum</t>
+          <t>Wessen</t>
         </is>
       </c>
       <c r="H61" s="2" t="n">
@@ -5583,7 +5583,7 @@
       </c>
       <c r="J74" s="2" t="inlineStr">
         <is>
-          <t>„Wen“ fragt nach dem Akkusativ-Objekt (Person/Sache).</t>
+          <t>„Wen“ fragt nach einer Person im Akkusativ.</t>
         </is>
       </c>
       <c r="K74" s="2" t="inlineStr">
@@ -6102,7 +6102,7 @@
       </c>
       <c r="C82" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">_____ ist das gut? </t>
+          <t>_____ ist dieses Tool gut?</t>
         </is>
       </c>
       <c r="D82" s="2" t="inlineStr">
@@ -7032,7 +7032,7 @@
       </c>
       <c r="J95" s="2" t="inlineStr">
         <is>
-          <t>„Wen“ fragt nach dem Akkusativ-Objekt (Person/Sache).</t>
+          <t>„Wen“ fragt nach einer Person im Akkusativ.</t>
         </is>
       </c>
       <c r="K95" s="2" t="inlineStr">
@@ -7068,7 +7068,7 @@
       </c>
       <c r="C96" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">_____ glaubst du? </t>
+          <t>_____ glaubst du bei dieser Geschichte?</t>
         </is>
       </c>
       <c r="D96" s="2" t="inlineStr">
@@ -8481,7 +8481,7 @@
       </c>
       <c r="J116" s="2" t="inlineStr">
         <is>
-          <t>„Wen“ fragt nach dem Akkusativ-Objekt (Person/Sache).</t>
+          <t>„Wen“ fragt nach einer Person im Akkusativ.</t>
         </is>
       </c>
       <c r="K116" s="2" t="inlineStr">
@@ -8724,7 +8724,7 @@
       </c>
       <c r="C120" s="2" t="inlineStr">
         <is>
-          <t>_____ lernst du das?</t>
+          <t>_____ brauchst du dieses Wissen?</t>
         </is>
       </c>
       <c r="D120" s="2" t="inlineStr">
@@ -9000,7 +9000,7 @@
       </c>
       <c r="C124" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">_____ lernst du das? </t>
+          <t>_____ lernst du das in diesem Kurs?</t>
         </is>
       </c>
       <c r="D124" s="2" t="inlineStr">
@@ -9552,7 +9552,7 @@
       </c>
       <c r="C132" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">_____ lachst du? </t>
+          <t>_____ lachst du so laut?</t>
         </is>
       </c>
       <c r="D132" s="2" t="inlineStr">
@@ -9572,7 +9572,7 @@
       </c>
       <c r="G132" s="2" t="inlineStr">
         <is>
-          <t>Worüber</t>
+          <t>Woher</t>
         </is>
       </c>
       <c r="H132" s="2" t="n">
@@ -9621,7 +9621,7 @@
       </c>
       <c r="C133" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">_____ machst du das? </t>
+          <t>_____ machst du das Schritt für Schritt?</t>
         </is>
       </c>
       <c r="D133" s="2" t="inlineStr">
@@ -9930,7 +9930,7 @@
       </c>
       <c r="J137" s="2" t="inlineStr">
         <is>
-          <t>„Wen“ fragt nach dem Akkusativ-Objekt (Person/Sache).</t>
+          <t>„Wen“ fragt nach einer Person im Akkusativ.</t>
         </is>
       </c>
       <c r="K137" s="2" t="inlineStr">
@@ -10794,7 +10794,7 @@
       </c>
       <c r="C150" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">_____ suchst du? </t>
+          <t>_____ suchst du im Wörterbuch?</t>
         </is>
       </c>
       <c r="D150" s="2" t="inlineStr">
@@ -11379,7 +11379,7 @@
       </c>
       <c r="J158" s="2" t="inlineStr">
         <is>
-          <t>„Wen“ fragt nach dem Akkusativ-Objekt (Person/Sache).</t>
+          <t>„Wen“ fragt nach einer Person im Akkusativ.</t>
         </is>
       </c>
       <c r="K158" s="2" t="inlineStr">
@@ -11898,7 +11898,7 @@
       </c>
       <c r="C166" s="2" t="inlineStr">
         <is>
-          <t>_____ ist der Termin?</t>
+          <t>_____ ist dieses Meeting gedacht?</t>
         </is>
       </c>
       <c r="D166" s="2" t="inlineStr">
@@ -12726,7 +12726,7 @@
       </c>
       <c r="C178" s="2" t="inlineStr">
         <is>
-          <t>_____ Tage kannst du?</t>
+          <t>_____ Tage kannst du teilnehmen?</t>
         </is>
       </c>
       <c r="D178" s="2" t="inlineStr">
@@ -12828,7 +12828,7 @@
       </c>
       <c r="J179" s="2" t="inlineStr">
         <is>
-          <t>„Wen“ fragt nach dem Akkusativ-Objekt (Person/Sache).</t>
+          <t>„Wen“ fragt nach einer Person im Akkusativ.</t>
         </is>
       </c>
       <c r="K179" s="2" t="inlineStr">
@@ -13899,12 +13899,12 @@
       </c>
       <c r="C195" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">_____ machst du eine Pause? </t>
+          <t>_____ machst du jetzt eine Pause?</t>
         </is>
       </c>
       <c r="D195" s="2" t="inlineStr">
         <is>
-          <t>Worauf</t>
+          <t>Wer</t>
         </is>
       </c>
       <c r="E195" s="2" t="inlineStr">
@@ -13914,12 +13914,12 @@
       </c>
       <c r="F195" s="2" t="inlineStr">
         <is>
-          <t>Wofür</t>
+          <t>Wem</t>
         </is>
       </c>
       <c r="G195" s="2" t="inlineStr">
         <is>
-          <t>Wann</t>
+          <t>Woran</t>
         </is>
       </c>
       <c r="H195" s="2" t="n">
@@ -14277,7 +14277,7 @@
       </c>
       <c r="J200" s="2" t="inlineStr">
         <is>
-          <t>„Wen“ fragt nach dem Akkusativ-Objekt (Person/Sache).</t>
+          <t>„Wen“ fragt nach einer Person im Akkusativ.</t>
         </is>
       </c>
       <c r="K200" s="2" t="inlineStr">
@@ -14934,7 +14934,7 @@
       </c>
       <c r="C210" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">_____ hast du Zeit? </t>
+          <t>_____ hast du im Projekt Zeit zu helfen?</t>
         </is>
       </c>
       <c r="D210" s="2" t="inlineStr">

</xml_diff>